<commit_message>
fixed normalization test and added library conversion
</commit_message>
<xml_diff>
--- a/backend/fms_core/tests/valid_templates/Library_conversion_v3_10_0.xlsx
+++ b/backend/fms_core/tests/valid_templates/Library_conversion_v3_10_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sballesteros/Documents/Freezeman/freezeman/backend/fms_core/tests/valid_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C42A67A-3CB0-EF4F-9CD9-05E2851ADC42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EFAE53-C7FE-4B44-963C-A8783B47BE88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" xr2:uid="{405E7239-1D14-6F47-A693-F6EDB1481B97}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15940" activeTab="1" xr2:uid="{405E7239-1D14-6F47-A693-F6EDB1481B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Conversion Batch" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="81">
   <si>
     <t>Template Version</t>
   </si>
@@ -336,6 +336,15 @@
   <si>
     <t>3.10.0</t>
   </si>
+  <si>
+    <t>SOURCECONTAINER4LIBRARYPOOLCONVERSION</t>
+  </si>
+  <si>
+    <t>Container4LibraryDest4</t>
+  </si>
+  <si>
+    <t>Library conversion comment 4</t>
+  </si>
 </sst>
 </file>
 
@@ -506,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -574,6 +583,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DBEF91C-DC9D-184F-9DE0-D7E7DAC2E4DD}">
   <dimension ref="A1:AMG387"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3106,12 +3116,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07BE83E-81BB-7B4B-B20C-1C27C9CCE468}">
   <dimension ref="A1:P484"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="40.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45" style="1" customWidth="1"/>
     <col min="4" max="4" width="32" style="1" customWidth="1"/>
     <col min="5" max="5" width="32.83203125" customWidth="1"/>
     <col min="6" max="6" width="35.1640625" customWidth="1"/>
@@ -3354,16 +3367,38 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="30"/>
+      <c r="A11" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="D11" s="30"/>
-      <c r="H11" s="32"/>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="32" t="s">
+        <v>12</v>
+      </c>
       <c r="J11" s="32"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="37"/>
+      <c r="K11" s="38">
+        <v>10</v>
+      </c>
+      <c r="L11" s="45">
+        <v>10</v>
+      </c>
       <c r="M11" s="34"/>
-      <c r="N11" s="35" t="str">
-        <f t="shared" ref="N11:N74" si="0">IF(M11,M11/K11, "" )</f>
-        <v/>
+      <c r="N11" s="35">
+        <v>5</v>
+      </c>
+      <c r="O11" s="45">
+        <v>5</v>
+      </c>
+      <c r="P11" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -3375,7 +3410,7 @@
       <c r="L12" s="37"/>
       <c r="M12" s="34"/>
       <c r="N12" s="35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="N11:N74" si="0">IF(M12,M12/K12, "" )</f>
         <v/>
       </c>
     </row>
@@ -9533,7 +9568,7 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>H11:H483</xm:sqref>
+          <xm:sqref>H12:H483</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{4AB5AF76-E211-634E-9AA8-992264C6DB7B}">
           <x14:formula1>
@@ -9557,7 +9592,7 @@
           <x14:formula1>
             <xm:f>Index!$E$2:$E$11</xm:f>
           </x14:formula1>
-          <xm:sqref>H8:H10</xm:sqref>
+          <xm:sqref>H8:H11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" xr:uid="{FE2119AA-4500-3E4B-929B-3FBDA54913E4}">
           <x14:formula1>

</xml_diff>